<commit_message>
update colores de graficos y datos del dashboard
</commit_message>
<xml_diff>
--- a/server/resources/data_dashboard.xlsx
+++ b/server/resources/data_dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Miguel/Desktop/khora/proyecto_visor_Privado_EMSV/Visor_Privado_EMSV/server/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29852584-C037-8B48-8DE6-FB0A639E41CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A414249-38E4-5247-96BC-7659BE17024E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{FF8EA80C-DBF0-45CC-B8AC-E813896C236E}"/>
+    <workbookView xWindow="2200" yWindow="1240" windowWidth="23260" windowHeight="12460" activeTab="2" xr2:uid="{FF8EA80C-DBF0-45CC-B8AC-E813896C236E}"/>
   </bookViews>
   <sheets>
     <sheet name="Info.Operativa" sheetId="1" r:id="rId1"/>
@@ -473,13 +473,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +800,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="157" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="157" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -856,7 +856,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="157" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -960,8 +960,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="157" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="157" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -974,8 +974,8 @@
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="22">
-        <v>3.7591625322701251E-2</v>
+      <c r="B1" s="24">
+        <v>3.7591625322701301</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1093,7 +1093,7 @@
       <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>272</v>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       <c r="A12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>147</v>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       <c r="A13" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>153</v>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
       <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>503</v>
       </c>
       <c r="C2" s="15">
@@ -1520,7 +1520,7 @@
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>144</v>
       </c>
       <c r="C3" s="15">

</xml_diff>